<commit_message>
melhorias na planilha e outros
</commit_message>
<xml_diff>
--- a/backend/resources/excel/Planilha_template.xlsx
+++ b/backend/resources/excel/Planilha_template.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Pagina1" sheetId="1" r:id="rId1"/>
-    <sheet name="Pagina2" sheetId="2" r:id="rId2"/>
+    <sheet name="Pagina2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+  <si>
+    <t>.</t>
+  </si>
   <si>
     <t>APROVAÇÃO</t>
   </si>
@@ -86,30 +89,6 @@
   <si>
     <t>DESENHISTA:</t>
   </si>
-  <si>
-    <t>Diretor Agrícola:___________________________________________________________________________________________</t>
-  </si>
-  <si>
-    <t>Topografia:______________________________________________________________________</t>
-  </si>
-  <si>
-    <t>Diretor Divisão Agrícola:________________________________________________________________________________</t>
-  </si>
-  <si>
-    <t>Preparo e Plantio:__________________________________________________________</t>
-  </si>
-  <si>
-    <t>Gerente Agrícola:_________________________________________________________________________</t>
-  </si>
-  <si>
-    <t>Colheita e Transporte:__________________________________________________________</t>
-  </si>
-  <si>
-    <t>Ger. de Preparo e Plantio:_______________________________________________________________</t>
-  </si>
-  <si>
-    <t>Irrigação - Fertirrigação:_____________________________________________________</t>
-  </si>
 </sst>
 </file>
 
@@ -121,7 +100,7 @@
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,12 +111,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -499,7 +472,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -564,23 +537,12 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,19 +564,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -650,12 +599,109 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -762,152 +808,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -916,101 +962,130 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1360,10 +1435,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K794"/>
+  <dimension ref="A1:Q794"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1382,20 +1457,20 @@
     <row r="2" ht="18.75" customHeight="1"/>
     <row r="3" ht="18.75" customHeight="1" spans="1:11">
       <c r="A3" s="2"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="26"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" ht="18.75" customHeight="1" spans="1:11">
       <c r="A4" s="5"/>
-      <c r="K4" s="28"/>
+      <c r="K4" s="25"/>
     </row>
     <row r="5" ht="18.75" customHeight="1" spans="1:11">
       <c r="A5" s="5"/>
@@ -1406,9 +1481,9 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="28"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="25"/>
     </row>
     <row r="6" ht="18.75" customHeight="1" spans="1:11">
       <c r="A6" s="5"/>
@@ -1419,9 +1494,9 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="28"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" ht="18.75" customHeight="1" spans="1:11">
       <c r="A7" s="5"/>
@@ -1432,9 +1507,9 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="28"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="25"/>
     </row>
     <row r="8" ht="18.75" customHeight="1" spans="1:11">
       <c r="A8" s="5"/>
@@ -1445,9 +1520,9 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="28"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="25"/>
     </row>
     <row r="9" ht="18.75" customHeight="1" spans="1:11">
       <c r="A9" s="5"/>
@@ -1458,9 +1533,9 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="28"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="25"/>
     </row>
     <row r="10" ht="18.75" customHeight="1" spans="1:11">
       <c r="A10" s="5"/>
@@ -1471,9 +1546,9 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="28"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="25"/>
     </row>
     <row r="11" ht="18.75" customHeight="1" spans="1:11">
       <c r="A11" s="5"/>
@@ -1482,11 +1557,11 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="34"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="28"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="25"/>
     </row>
     <row r="12" ht="19.5" customHeight="1" spans="1:11">
       <c r="A12" s="5"/>
@@ -1497,9 +1572,9 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="28"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="25"/>
     </row>
     <row r="13" ht="19.5" customHeight="1" spans="1:11">
       <c r="A13" s="5"/>
@@ -1510,9 +1585,9 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="28"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="25"/>
     </row>
     <row r="14" ht="19.5" customHeight="1" spans="1:11">
       <c r="A14" s="5"/>
@@ -1523,9 +1598,9 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="28"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="25"/>
     </row>
     <row r="15" ht="19.5" customHeight="1" spans="1:11">
       <c r="A15" s="5"/>
@@ -1536,9 +1611,9 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="28"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="25"/>
     </row>
     <row r="16" ht="19.5" customHeight="1" spans="1:11">
       <c r="A16" s="5"/>
@@ -1549,9 +1624,9 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="28"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="25"/>
     </row>
     <row r="17" ht="19.5" customHeight="1" spans="1:11">
       <c r="A17" s="5"/>
@@ -1562,9 +1637,9 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="28"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="25"/>
     </row>
     <row r="18" ht="19.5" customHeight="1" spans="1:11">
       <c r="A18" s="5"/>
@@ -1577,7 +1652,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="27"/>
+      <c r="K18" s="26"/>
     </row>
     <row r="19" ht="19.5" customHeight="1" spans="1:11">
       <c r="A19" s="5"/>
@@ -1590,7 +1665,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-      <c r="K19" s="27"/>
+      <c r="K19" s="26"/>
     </row>
     <row r="20" ht="19.5" customHeight="1" spans="1:11">
       <c r="A20" s="5"/>
@@ -1603,7 +1678,7 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="27"/>
+      <c r="K20" s="26"/>
     </row>
     <row r="21" ht="19.5" customHeight="1" spans="1:11">
       <c r="A21" s="5"/>
@@ -1616,7 +1691,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="27"/>
+      <c r="K21" s="26"/>
     </row>
     <row r="22" ht="19.5" customHeight="1" spans="1:11">
       <c r="A22" s="5"/>
@@ -1629,7 +1704,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="27"/>
+      <c r="K22" s="26"/>
     </row>
     <row r="23" ht="19.5" customHeight="1" spans="1:11">
       <c r="A23" s="5"/>
@@ -1642,7 +1717,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="27"/>
+      <c r="K23" s="26"/>
     </row>
     <row r="24" ht="19.5" customHeight="1" spans="1:11">
       <c r="A24" s="5"/>
@@ -1655,7 +1730,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="27"/>
+      <c r="K24" s="26"/>
     </row>
     <row r="25" ht="19.5" customHeight="1" spans="1:11">
       <c r="A25" s="5"/>
@@ -1668,7 +1743,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="27"/>
+      <c r="K25" s="26"/>
     </row>
     <row r="26" ht="18.75" customHeight="1" spans="1:11">
       <c r="A26" s="5"/>
@@ -1681,9 +1756,9 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="27"/>
-    </row>
-    <row r="27" ht="19.5" customHeight="1" spans="1:11">
+      <c r="K26" s="26"/>
+    </row>
+    <row r="27" ht="19.5" customHeight="1" spans="1:17">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1694,7 +1769,10 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
-      <c r="K27" s="27"/>
+      <c r="K27" s="26"/>
+      <c r="Q27" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" ht="19.5" customHeight="1" spans="1:11">
       <c r="A28" s="5"/>
@@ -1707,7 +1785,7 @@
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="27"/>
+      <c r="K28" s="26"/>
     </row>
     <row r="29" ht="19.5" customHeight="1" spans="1:11">
       <c r="A29" s="5"/>
@@ -1720,136 +1798,136 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="27"/>
+      <c r="K29" s="26"/>
     </row>
     <row r="30" ht="19.5" customHeight="1" spans="1:11">
-      <c r="A30" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="29"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="44"/>
     </row>
     <row r="31" ht="18.75" customHeight="1" spans="1:11">
-      <c r="A31" s="10" t="s">
-        <v>2</v>
+      <c r="A31" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="B31" s="6"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="10" t="s">
-        <v>3</v>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="10" t="s">
-        <v>4</v>
+      <c r="H31" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="I31" s="7"/>
-      <c r="J31" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K31" s="31"/>
+      <c r="J31" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="K31" s="46"/>
     </row>
     <row r="32" ht="19.5" customHeight="1" spans="1:11">
-      <c r="A32" s="10" t="s">
-        <v>6</v>
+      <c r="A32" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="B32" s="6"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="10" t="s">
-        <v>7</v>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="10" t="s">
-        <v>8</v>
+      <c r="H32" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="I32" s="7"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="31"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="46"/>
     </row>
     <row r="33" ht="18.75" customHeight="1" spans="1:11">
-      <c r="A33" s="10" t="s">
-        <v>9</v>
+      <c r="A33" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="B33" s="6"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="10" t="s">
-        <v>10</v>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="10" t="s">
-        <v>11</v>
+      <c r="H33" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="I33" s="7"/>
-      <c r="J33" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="K33" s="31"/>
+      <c r="J33" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" s="46"/>
     </row>
     <row r="34" ht="15.75" customHeight="1" spans="1:11">
-      <c r="A34" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="14" t="s">
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I34" s="15"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="33"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="14"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="50"/>
     </row>
     <row r="35" ht="15.75" customHeight="1" spans="1:11">
-      <c r="A35" s="17"/>
-      <c r="B35" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="19" t="s">
+      <c r="A35" s="15"/>
+      <c r="B35" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="20"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="22" t="s">
+      <c r="C35" s="4"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="21"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="17"/>
     </row>
     <row r="36" ht="22" customHeight="1" spans="1:11">
-      <c r="A36" s="23"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="24"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="21"/>
     </row>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
@@ -2627,27 +2705,40 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J687"/>
+  <dimension ref="A1:W794"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.152380952381" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7238095238095" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.0095238095238" style="1" customWidth="1"/>
-    <col min="4" max="5" width="12.5809523809524" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.152380952381" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.4380952380952" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.2952380952381" style="1" customWidth="1"/>
-    <col min="9" max="10" width="12.5809523809524" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.8666666666667" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.0095238095238" style="1" customWidth="1"/>
+    <col min="6" max="7" width="12.5809523809524" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.152380952381" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1428571428571" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7142857142857" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85714285714286" style="1" customWidth="1"/>
+    <col min="12" max="15" width="8.57142857142857" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.42857142857143" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1"/>
+    <row r="1" ht="18.75" customHeight="1" spans="9:16">
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" ht="18.75" customHeight="1"/>
-    <row r="3" ht="18.75" customHeight="1" spans="1:10">
+    <row r="3" ht="18.75" customHeight="1" spans="1:16">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2655,340 +2746,661 @@
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="26"/>
-    </row>
-    <row r="4" ht="18.75" customHeight="1" spans="1:10">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="23"/>
+    </row>
+    <row r="4" ht="18.75" customHeight="1" spans="1:16">
       <c r="A4" s="5"/>
-      <c r="F4" s="6"/>
-      <c r="J4" s="27"/>
-    </row>
-    <row r="5" ht="18.75" customHeight="1" spans="1:10">
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="25"/>
+    </row>
+    <row r="5" ht="18.75" customHeight="1" spans="1:16">
       <c r="A5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="J5" s="27"/>
-    </row>
-    <row r="6" ht="18.75" customHeight="1" spans="1:10">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="25"/>
+    </row>
+    <row r="6" ht="18.75" customHeight="1" spans="1:16">
       <c r="A6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="27"/>
-    </row>
-    <row r="7" ht="18.75" customHeight="1" spans="1:10">
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="25"/>
+    </row>
+    <row r="7" ht="18.75" customHeight="1" spans="1:16">
       <c r="A7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="27"/>
-    </row>
-    <row r="8" ht="18.75" customHeight="1" spans="1:10">
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="25"/>
+    </row>
+    <row r="8" ht="18.75" customHeight="1" spans="1:16">
       <c r="A8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="28"/>
-    </row>
-    <row r="9" ht="18.75" customHeight="1" spans="1:10">
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="25"/>
+    </row>
+    <row r="9" ht="18.75" customHeight="1" spans="1:16">
       <c r="A9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="27"/>
-    </row>
-    <row r="10" ht="18.75" customHeight="1" spans="1:10">
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="25"/>
+    </row>
+    <row r="10" ht="18.75" customHeight="1" spans="1:16">
       <c r="A10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="27"/>
-    </row>
-    <row r="11" ht="18.75" customHeight="1" spans="1:10">
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="25"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1" spans="1:21">
       <c r="A11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="27"/>
-    </row>
-    <row r="12" ht="18.75" customHeight="1" spans="1:10">
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="25"/>
+      <c r="U11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" ht="19.5" customHeight="1" spans="1:16">
       <c r="A12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="27"/>
-    </row>
-    <row r="13" ht="18.75" customHeight="1" spans="1:10">
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="25"/>
+    </row>
+    <row r="13" ht="19.5" customHeight="1" spans="1:16">
       <c r="A13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="27"/>
-    </row>
-    <row r="14" ht="18.75" customHeight="1" spans="1:10">
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="25"/>
+    </row>
+    <row r="14" ht="19.5" customHeight="1" spans="1:16">
       <c r="A14" s="5"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="27"/>
-    </row>
-    <row r="15" ht="18.75" customHeight="1" spans="1:10">
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="25"/>
+    </row>
+    <row r="15" ht="19.5" customHeight="1" spans="1:16">
       <c r="A15" s="5"/>
-      <c r="J15" s="27"/>
-    </row>
-    <row r="16" ht="18.75" customHeight="1" spans="1:10">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="25"/>
+    </row>
+    <row r="16" ht="19.5" customHeight="1" spans="1:16">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="J16" s="27"/>
-    </row>
-    <row r="17" ht="18.75" customHeight="1" spans="1:10">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="25"/>
+    </row>
+    <row r="17" ht="19.5" customHeight="1" spans="1:16">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="J17" s="27"/>
-    </row>
-    <row r="18" ht="18.75" customHeight="1" spans="1:10">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="25"/>
+    </row>
+    <row r="18" ht="19.5" customHeight="1" spans="1:16">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="J18" s="27"/>
-    </row>
-    <row r="19" ht="18.75" customHeight="1" spans="1:10">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="26"/>
+    </row>
+    <row r="19" ht="19.5" customHeight="1" spans="1:16">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="J19" s="27"/>
-    </row>
-    <row r="20" ht="18.75" customHeight="1" spans="1:10">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="26"/>
+    </row>
+    <row r="20" ht="19.5" customHeight="1" spans="1:16">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="J20" s="27"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1" spans="1:10">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="26"/>
+    </row>
+    <row r="21" ht="19.5" customHeight="1" spans="1:16">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="J21" s="27"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" spans="1:10">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="26"/>
+    </row>
+    <row r="22" ht="19.5" customHeight="1" spans="1:16">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="J22" s="27"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1" spans="1:10">
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="26"/>
+    </row>
+    <row r="23" ht="19.5" customHeight="1" spans="1:16">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="J23" s="27"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1" spans="1:10">
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="26"/>
+    </row>
+    <row r="24" ht="19.5" customHeight="1" spans="1:16">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="J24" s="27"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1" spans="1:10">
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="26"/>
+    </row>
+    <row r="25" ht="19.5" customHeight="1" spans="1:16">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="27"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1" spans="1:10">
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="26"/>
+    </row>
+    <row r="26" ht="18.75" customHeight="1" spans="1:16">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="27"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1" spans="1:10">
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="26"/>
+    </row>
+    <row r="27" ht="19.5" customHeight="1" spans="1:23">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
-      <c r="J27" s="27"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1" spans="1:10">
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="26"/>
+      <c r="W27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" ht="19.5" customHeight="1" spans="1:16">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
-      <c r="J28" s="27"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1" spans="1:10">
-      <c r="A29" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="8" t="s">
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="26"/>
+    </row>
+    <row r="29" ht="19.5" customHeight="1" spans="1:16">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="26"/>
+    </row>
+    <row r="30" ht="19.5" customHeight="1" spans="1:16">
+      <c r="A30" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="29"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1" spans="1:10">
-      <c r="A30" s="10" t="s">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="28"/>
+    </row>
+    <row r="31" ht="18.75" customHeight="1" spans="1:17">
+      <c r="A31" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="7"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" s="8"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="43"/>
+    </row>
+    <row r="32" ht="19.5" customHeight="1" spans="1:17">
+      <c r="A32" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32" s="7"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="43"/>
+    </row>
+    <row r="33" ht="18.75" customHeight="1" spans="1:17">
+      <c r="A33" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="L33" s="35"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="43"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1" spans="1:17">
+      <c r="A34" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="14"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="43"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1" spans="1:16">
+      <c r="A35" s="15"/>
+      <c r="B35" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G30" s="7"/>
-      <c r="H30" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I30" s="30"/>
-      <c r="J30" s="31"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1" spans="1:10">
-      <c r="A31" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="31"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1" spans="1:10">
-      <c r="A32" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="7"/>
-      <c r="H32" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I32" s="30"/>
-      <c r="J32" s="31"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1" spans="1:10">
-      <c r="A33" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="15"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="33"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1" spans="1:10">
-      <c r="A34" s="17"/>
-      <c r="B34" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="21"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1" spans="1:10">
-      <c r="A35" s="23"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="24"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="25"/>
+    </row>
+    <row r="36" ht="22" customHeight="1" spans="1:16">
+      <c r="A36" s="20"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="21"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" spans="12:18">
+      <c r="L37" s="42"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="42"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="42"/>
+      <c r="Q37" s="42"/>
+      <c r="R37" s="42"/>
+    </row>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1"/>
@@ -3639,12 +4051,122 @@
     <row r="685" ht="15.75" customHeight="1"/>
     <row r="686" ht="15.75" customHeight="1"/>
     <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="F29:J29"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:J34"/>
+  <mergeCells count="7">
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="H30:P30"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:P35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>